<commit_message>
-inf fix on keepers
</commit_message>
<xml_diff>
--- a/data/DreamLeague23-24.xlsx
+++ b/data/DreamLeague23-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kelloggcompany-my.sharepoint.com/personal/bryn_coombe_kellogg_com/Documents/Desktop/Dream League/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\git\dreamleague\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="8_{2143D4C5-D5B5-4416-B5A6-A1B2D5502F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B4717F7-D007-48D4-8661-19F1FB9DC31D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DFD8AE-238C-4BF7-9D73-72BAB152ED2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Table" sheetId="3" r:id="rId3"/>
     <sheet name="Cup" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="327">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -991,6 +991,30 @@
   </si>
   <si>
     <t>MACAULEY LANGSTAFF</t>
+  </si>
+  <si>
+    <t>CHRIS LONG</t>
+  </si>
+  <si>
+    <t>CREWE</t>
+  </si>
+  <si>
+    <t>JAKE YOUNG</t>
+  </si>
+  <si>
+    <t>JONATHAN ROWE</t>
+  </si>
+  <si>
+    <t>MARTYN WAGHORN</t>
+  </si>
+  <si>
+    <t>SOLLY MARCH</t>
+  </si>
+  <si>
+    <t>WATFORD</t>
+  </si>
+  <si>
+    <t>WILL EVANS</t>
   </si>
 </sst>
 </file>
@@ -1727,9 +1751,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1738,6 +1759,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2929,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IX377"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16:O16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A137" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3049,13 +3073,13 @@
       <c r="O4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="116" t="s">
+      <c r="R4" s="115" t="s">
         <v>287</v>
       </c>
-      <c r="S4" s="116"/>
-      <c r="T4" s="116"/>
-      <c r="U4" s="116"/>
-      <c r="V4" s="116"/>
+      <c r="S4" s="115"/>
+      <c r="T4" s="115"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="115"/>
     </row>
     <row r="5" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="83"/>
@@ -3070,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="87"/>
       <c r="H5" s="88"/>
@@ -3090,25 +3114,25 @@
       </c>
       <c r="N5" s="19">
         <f>SUM(F8:F25)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O5" s="20">
         <f>SUM(F5:F7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R5" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="115">
+      <c r="S5" s="114">
         <f>_xlfn.XLOOKUP(R5,K:K,M:M)</f>
         <v>3</v>
       </c>
-      <c r="T5" s="114" t="s">
+      <c r="T5" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U5" s="115">
+      <c r="U5" s="114">
         <f>_xlfn.XLOOKUP(V5,K:K,M:M)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5" s="81" t="s">
         <v>224</v>
@@ -3135,11 +3159,11 @@
       </c>
       <c r="M6" s="25">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="N6" s="26">
         <f>SUM(F35:F52)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O6" s="27">
         <f>SUM(F32:F34)</f>
@@ -3148,14 +3172,14 @@
       <c r="R6" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="S6" s="115">
+      <c r="S6" s="114">
         <f>_xlfn.XLOOKUP(R6,K:K,M:M)</f>
         <v>3</v>
       </c>
-      <c r="T6" s="114" t="s">
+      <c r="T6" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U6" s="115">
+      <c r="U6" s="114">
         <f>_xlfn.XLOOKUP(V6,K:K,M:M)</f>
         <v>4</v>
       </c>
@@ -3188,25 +3212,25 @@
       </c>
       <c r="N7" s="26">
         <f>SUM(F62:F79)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O7" s="27">
         <f>SUM(F59:F61)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="115">
+      <c r="S7" s="114">
         <f>_xlfn.XLOOKUP(R7,K:K,M:M)</f>
         <v>3</v>
       </c>
-      <c r="T7" s="114" t="s">
+      <c r="T7" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U7" s="115">
+      <c r="U7" s="114">
         <f>_xlfn.XLOOKUP(V7,K:K,M:M)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="V7" s="81" t="s">
         <v>34</v>
@@ -3242,11 +3266,11 @@
       </c>
       <c r="M8" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N8" s="26">
         <f>SUM(F89:F106)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="O8" s="27">
         <f>SUM(F86:F88)</f>
@@ -3284,11 +3308,11 @@
       </c>
       <c r="M9" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N9" s="77">
         <f>SUM(F116:F133)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="O9" s="78">
         <f>SUM(F113:F115)</f>
@@ -3316,43 +3340,47 @@
       </c>
       <c r="M10" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N10" s="26">
         <f>SUM(F143:F160)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O10" s="27">
         <f>SUM(F140:F142)</f>
-        <v>6</v>
-      </c>
-      <c r="R10" s="116" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="115" t="s">
         <v>288</v>
       </c>
-      <c r="S10" s="116"/>
-      <c r="T10" s="116"/>
-      <c r="U10" s="116"/>
-      <c r="V10" s="116"/>
+      <c r="S10" s="115"/>
+      <c r="T10" s="115"/>
+      <c r="U10" s="115"/>
+      <c r="V10" s="115"/>
     </row>
     <row r="11" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="83"/>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="103" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="104">
         <v>17</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="105">
         <v>1</v>
       </c>
-      <c r="G11" s="87"/>
-      <c r="H11" s="88"/>
+      <c r="G11" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="H11" s="88">
+        <v>45169</v>
+      </c>
       <c r="I11" s="110"/>
       <c r="J11" s="86"/>
       <c r="K11" s="23" t="str">
@@ -3369,23 +3397,23 @@
       </c>
       <c r="N11" s="26">
         <f>SUM(F170:F187)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O11" s="27">
         <f>SUM(F167:F169)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R11" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="S11" s="115">
+      <c r="S11" s="114">
         <f>SUM(F11:F15)</f>
-        <v>2</v>
-      </c>
-      <c r="T11" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="T11" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U11" s="115">
+      <c r="U11" s="114">
         <f>SUM(F227:F231)</f>
         <v>1</v>
       </c>
@@ -3399,18 +3427,20 @@
         <v>18</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>104</v>
+        <v>324</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="29">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>284</v>
       </c>
       <c r="F12" s="30">
-        <v>1</v>
-      </c>
-      <c r="G12" s="92"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="92">
+        <v>45169</v>
+      </c>
       <c r="H12" s="88"/>
       <c r="I12" s="110"/>
       <c r="J12" s="86"/>
@@ -3424,15 +3454,15 @@
       </c>
       <c r="M12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="77">
         <f>SUM(F197:F214)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" s="78">
         <f>SUM(F194:F196)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -3441,19 +3471,19 @@
         <v>18</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>163</v>
+        <v>104</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="E13" s="29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="92"/>
-      <c r="H13" s="79"/>
+      <c r="H13" s="88"/>
       <c r="I13" s="110"/>
       <c r="J13" s="86"/>
       <c r="K13" s="75" t="str">
@@ -3466,33 +3496,47 @@
       </c>
       <c r="M13" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="77">
         <f>SUM(F224:F241)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O13" s="78">
         <f>SUM(F221:F223)</f>
-        <v>5</v>
-      </c>
-      <c r="R13" s="116" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="115" t="s">
         <v>289</v>
       </c>
-      <c r="S13" s="116"/>
-      <c r="T13" s="116"/>
-      <c r="U13" s="116"/>
-      <c r="V13" s="116"/>
+      <c r="S13" s="115"/>
+      <c r="T13" s="115"/>
+      <c r="U13" s="115"/>
+      <c r="V13" s="115"/>
     </row>
     <row r="14" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="83"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="88"/>
+      <c r="B14" s="103" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="103" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="103" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="104">
+        <v>2</v>
+      </c>
+      <c r="F14" s="105">
+        <v>0</v>
+      </c>
+      <c r="G14" s="92" t="s">
+        <v>285</v>
+      </c>
+      <c r="H14" s="88">
+        <v>45162</v>
+      </c>
       <c r="I14" s="110"/>
       <c r="J14" s="83"/>
       <c r="K14" s="75" t="str">
@@ -3509,25 +3553,25 @@
       </c>
       <c r="N14" s="77">
         <f>SUM(F251:F268)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O14" s="78">
         <f>SUM(F248:F250)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R14" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="S14" s="115">
+      <c r="S14" s="114">
         <f>_xlfn.XLOOKUP(R14,C:C,F:F)</f>
         <v>1</v>
       </c>
-      <c r="T14" s="114" t="s">
+      <c r="T14" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U14" s="115">
+      <c r="U14" s="114">
         <f>_xlfn.XLOOKUP(V14,C:C,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V14" s="81" t="s">
         <v>232</v>
@@ -3535,12 +3579,24 @@
     </row>
     <row r="15" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="83"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="92"/>
+      <c r="B15" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="F15" s="30">
+        <v>1</v>
+      </c>
+      <c r="G15" s="92">
+        <v>45162</v>
+      </c>
       <c r="H15" s="88"/>
       <c r="I15" s="110"/>
       <c r="J15" s="86"/>
@@ -3554,11 +3610,11 @@
       </c>
       <c r="M15" s="25">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N15" s="26">
         <f>SUM(F277:F295)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O15" s="27">
         <f>SUM(F275:F276)</f>
@@ -3606,11 +3662,11 @@
       </c>
       <c r="N16" s="26">
         <f>SUM(F305:F322)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O16" s="27">
         <f>SUM(F302:F304)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -3648,23 +3704,23 @@
       </c>
       <c r="M17" s="25">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="N17" s="26">
         <f>SUM(F332:F349)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O17" s="27">
         <f>SUM(F329:F331)</f>
-        <v>9</v>
-      </c>
-      <c r="R17" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="R17" s="115" t="s">
         <v>292</v>
       </c>
-      <c r="S17" s="116"/>
-      <c r="T17" s="116"/>
-      <c r="U17" s="116"/>
-      <c r="V17" s="116"/>
+      <c r="S17" s="115"/>
+      <c r="T17" s="115"/>
+      <c r="U17" s="115"/>
+      <c r="V17" s="115"/>
     </row>
     <row r="18" spans="1:22" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="83"/>
@@ -3699,29 +3755,29 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" ref="M18" si="1">N18-O18</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18" s="26">
         <f>SUM(F359:F376)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O18" s="27">
         <f>SUM(F356:F358)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R18" s="81" t="s">
         <v>301</v>
       </c>
-      <c r="S18" s="115">
+      <c r="S18" s="114">
         <f>_xlfn.XLOOKUP(R18,K:K,O:O)</f>
-        <v>2</v>
-      </c>
-      <c r="T18" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="T18" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U18" s="115">
+      <c r="U18" s="114">
         <f>_xlfn.XLOOKUP(V18,K:K,O:O)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V18" s="81" t="s">
         <v>46</v>
@@ -3784,35 +3840,37 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="R20" s="116" t="s">
+      <c r="R20" s="115" t="s">
         <v>293</v>
       </c>
-      <c r="S20" s="116"/>
-      <c r="T20" s="116"/>
-      <c r="U20" s="116"/>
-      <c r="V20" s="116"/>
+      <c r="S20" s="115"/>
+      <c r="T20" s="115"/>
+      <c r="U20" s="115"/>
+      <c r="V20" s="115"/>
     </row>
     <row r="21" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="83"/>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="103" t="s">
         <v>306</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="104" t="s">
         <v>284</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="105">
         <v>0</v>
       </c>
       <c r="G21" s="92">
         <v>45155</v>
       </c>
-      <c r="H21" s="88"/>
+      <c r="H21" s="88">
+        <v>45169</v>
+      </c>
       <c r="I21" s="110"/>
       <c r="J21" s="80"/>
       <c r="K21" s="1"/>
@@ -3823,16 +3881,16 @@
       <c r="R21" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="S21" s="115">
+      <c r="S21" s="114">
         <f>_xlfn.XLOOKUP(R22,C:C,F:F)</f>
         <v>1</v>
       </c>
-      <c r="T21" s="114" t="s">
+      <c r="T21" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U21" s="115">
+      <c r="U21" s="114">
         <f>_xlfn.XLOOKUP(V22,C:C,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V21" s="81" t="s">
         <v>70</v>
@@ -3844,18 +3902,20 @@
         <v>19</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>165</v>
+        <v>323</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" s="29">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>284</v>
       </c>
       <c r="F22" s="30">
         <v>0</v>
       </c>
-      <c r="G22" s="92"/>
+      <c r="G22" s="92">
+        <v>45169</v>
+      </c>
       <c r="H22" s="79"/>
       <c r="I22" s="94"/>
       <c r="J22" s="80"/>
@@ -3873,11 +3933,21 @@
     </row>
     <row r="23" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="83"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="105"/>
+      <c r="B23" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="29">
+        <v>1</v>
+      </c>
+      <c r="F23" s="30">
+        <v>0</v>
+      </c>
       <c r="G23" s="92"/>
       <c r="H23" s="88"/>
       <c r="I23" s="94"/>
@@ -3904,13 +3974,13 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="R24" s="116" t="s">
+      <c r="R24" s="115" t="s">
         <v>294</v>
       </c>
-      <c r="S24" s="116"/>
-      <c r="T24" s="116"/>
-      <c r="U24" s="116"/>
-      <c r="V24" s="116"/>
+      <c r="S24" s="115"/>
+      <c r="T24" s="115"/>
+      <c r="U24" s="115"/>
+      <c r="V24" s="115"/>
     </row>
     <row r="25" spans="1:22" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="83"/>
@@ -3931,16 +4001,16 @@
       <c r="R25" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="S25" s="115">
+      <c r="S25" s="114">
         <f>(_xlfn.XLOOKUP(R25,K:K,M:M))-(_xlfn.XLOOKUP(R26,C:C,F:F))</f>
-        <v>-5</v>
-      </c>
-      <c r="T25" s="114" t="s">
+        <v>-2</v>
+      </c>
+      <c r="T25" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="U25" s="115">
+      <c r="U25" s="114">
         <f>(_xlfn.XLOOKUP(V25,K:K,M:M))-(_xlfn.XLOOKUP(V26,C:C,F:F))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="V25" s="81" t="s">
         <v>70</v>
@@ -4008,13 +4078,13 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="R28" s="116" t="s">
+      <c r="R28" s="115" t="s">
         <v>295</v>
       </c>
-      <c r="S28" s="116"/>
-      <c r="T28" s="116"/>
-      <c r="U28" s="116"/>
-      <c r="V28" s="116"/>
+      <c r="S28" s="115"/>
+      <c r="T28" s="115"/>
+      <c r="U28" s="115"/>
+      <c r="V28" s="115"/>
     </row>
     <row r="29" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
@@ -4108,7 +4178,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="13"/>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="116" t="s">
         <v>17</v>
       </c>
       <c r="E32" s="14">
@@ -4117,8 +4187,12 @@
       <c r="F32" s="15">
         <v>8</v>
       </c>
-      <c r="G32" s="84"/>
-      <c r="H32" s="99"/>
+      <c r="G32" s="84" t="s">
+        <v>285</v>
+      </c>
+      <c r="H32" s="99">
+        <v>45169</v>
+      </c>
       <c r="I32" s="100"/>
       <c r="J32" s="80"/>
       <c r="K32" s="1"/>
@@ -4136,12 +4210,22 @@
     </row>
     <row r="33" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="83"/>
-      <c r="B33" s="21"/>
+      <c r="B33" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="90"/>
+      <c r="D33" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="F33" s="21">
+        <v>0</v>
+      </c>
+      <c r="G33" s="90">
+        <v>45169</v>
+      </c>
       <c r="H33" s="97"/>
       <c r="I33" s="98"/>
       <c r="J33" s="80"/>
@@ -4293,13 +4377,13 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="R38" s="116" t="s">
+      <c r="R38" s="115" t="s">
         <v>296</v>
       </c>
-      <c r="S38" s="116"/>
-      <c r="T38" s="116"/>
-      <c r="U38" s="116"/>
-      <c r="V38" s="116"/>
+      <c r="S38" s="115"/>
+      <c r="T38" s="115"/>
+      <c r="U38" s="115"/>
+      <c r="V38" s="115"/>
     </row>
     <row r="39" spans="1:22" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="83"/>
@@ -4316,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="95"/>
@@ -4444,7 +4528,7 @@
         <v>90</v>
       </c>
       <c r="F43" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G43" s="87"/>
       <c r="H43" s="92"/>
@@ -4557,10 +4641,10 @@
       <c r="F46" s="105">
         <v>0</v>
       </c>
-      <c r="G46" s="113" t="s">
+      <c r="G46" s="96" t="s">
         <v>285</v>
       </c>
-      <c r="H46" s="113">
+      <c r="H46" s="96">
         <v>45148</v>
       </c>
       <c r="I46" s="94"/>
@@ -4635,7 +4719,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="96"/>
@@ -4776,7 +4860,7 @@
       </c>
       <c r="F53" s="38">
         <f>SUM(F35:F52)-SUM(F32:F34)</f>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="G53" s="84"/>
       <c r="H53" s="97"/>
@@ -4877,7 +4961,7 @@
       </c>
       <c r="S56" s="81">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V56" s="81" t="s">
         <v>224</v>
@@ -4960,7 +5044,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G59" s="84"/>
       <c r="H59" s="97"/>
@@ -5003,7 +5087,7 @@
       </c>
       <c r="S60" s="81">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V60" s="81" t="s">
         <v>46</v>
@@ -5152,7 +5236,7 @@
         <v>30</v>
       </c>
       <c r="F65" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="87"/>
       <c r="H65" s="95"/>
@@ -5168,7 +5252,7 @@
       </c>
       <c r="S65" s="81">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V65" s="81" t="s">
         <v>24</v>
@@ -5296,7 +5380,7 @@
       </c>
       <c r="S69" s="81">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V69" s="81" t="s">
         <v>24</v>
@@ -5805,7 +5889,7 @@
         <v>13</v>
       </c>
       <c r="F92" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G92" s="87"/>
       <c r="H92" s="96"/>
@@ -5832,7 +5916,7 @@
         <v>6</v>
       </c>
       <c r="F93" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G93" s="92"/>
       <c r="H93" s="96"/>
@@ -6040,7 +6124,7 @@
         <v>12</v>
       </c>
       <c r="F101" s="30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G101" s="87"/>
       <c r="H101" s="96"/>
@@ -6067,7 +6151,7 @@
         <v>10</v>
       </c>
       <c r="F102" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G102" s="92"/>
       <c r="H102" s="96"/>
@@ -6168,7 +6252,7 @@
       </c>
       <c r="F107" s="38">
         <f>SUM(F89:F106)-SUM(F86:F88)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G107" s="84"/>
       <c r="H107" s="97"/>
@@ -6424,7 +6508,7 @@
         <v>15</v>
       </c>
       <c r="F119" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G119" s="87"/>
       <c r="H119" s="96"/>
@@ -6509,7 +6593,7 @@
         <v>284</v>
       </c>
       <c r="F122" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G122" s="92">
         <v>45155</v>
@@ -6555,7 +6639,7 @@
         <v>35</v>
       </c>
       <c r="F124" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G124" s="90"/>
       <c r="H124" s="99"/>
@@ -6636,7 +6720,7 @@
         <v>1</v>
       </c>
       <c r="F127" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G127" s="92"/>
       <c r="H127" s="96"/>
@@ -6771,7 +6855,7 @@
       </c>
       <c r="F134" s="38">
         <f>SUM(F116:F133)-SUM(F113:F115)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G134" s="84"/>
       <c r="H134" s="97"/>
@@ -6895,7 +6979,7 @@
         <v>3</v>
       </c>
       <c r="F140" s="15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G140" s="84"/>
       <c r="H140" s="99"/>
@@ -7136,13 +7220,13 @@
         <v>92</v>
       </c>
       <c r="D151" s="28" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="E151" s="29">
         <v>34</v>
       </c>
       <c r="F151" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G151" s="87"/>
       <c r="H151" s="96"/>
@@ -7240,10 +7324,10 @@
       <c r="B155" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C155" s="28" t="s">
+      <c r="C155" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="D155" s="28" t="s">
+      <c r="D155" s="103" t="s">
         <v>308</v>
       </c>
       <c r="E155" s="29">
@@ -7252,8 +7336,12 @@
       <c r="F155" s="30">
         <v>0</v>
       </c>
-      <c r="G155" s="92"/>
-      <c r="H155" s="96"/>
+      <c r="G155" s="92" t="s">
+        <v>285</v>
+      </c>
+      <c r="H155" s="96">
+        <v>45169</v>
+      </c>
       <c r="I155" s="95"/>
       <c r="J155" s="80"/>
       <c r="K155" s="1"/>
@@ -7264,12 +7352,24 @@
     </row>
     <row r="156" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="83"/>
-      <c r="B156" s="28"/>
-      <c r="C156" s="103"/>
-      <c r="D156" s="103"/>
-      <c r="E156" s="104"/>
-      <c r="F156" s="105"/>
-      <c r="G156" s="87"/>
+      <c r="B156" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C156" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="D156" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E156" s="104" t="s">
+        <v>284</v>
+      </c>
+      <c r="F156" s="105">
+        <v>0</v>
+      </c>
+      <c r="G156" s="92">
+        <v>45169</v>
+      </c>
       <c r="H156" s="96"/>
       <c r="I156" s="95"/>
       <c r="J156" s="80"/>
@@ -7358,7 +7458,7 @@
       </c>
       <c r="F161" s="38">
         <f>SUM(F143:F160)-SUM(F140:F142)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G161" s="84"/>
       <c r="H161" s="97"/>
@@ -7482,7 +7582,7 @@
         <v>4</v>
       </c>
       <c r="F167" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G167" s="84"/>
       <c r="H167" s="99"/>
@@ -7756,7 +7856,7 @@
         <v>1</v>
       </c>
       <c r="F179" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G179" s="87"/>
       <c r="H179" s="96"/>
@@ -8069,7 +8169,7 @@
         <v>2</v>
       </c>
       <c r="F194" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G194" s="84"/>
       <c r="H194" s="99"/>
@@ -8424,7 +8524,7 @@
         <v>1</v>
       </c>
       <c r="F209" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G209" s="92"/>
       <c r="H209" s="96"/>
@@ -8532,7 +8632,7 @@
       </c>
       <c r="F215" s="38">
         <f>SUM(F197:F214)-SUM(F194:F196)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G215" s="84"/>
       <c r="H215" s="97"/>
@@ -8649,17 +8749,21 @@
         <v>13</v>
       </c>
       <c r="C221" s="112"/>
-      <c r="D221" s="12" t="s">
+      <c r="D221" s="116" t="s">
         <v>204</v>
       </c>
       <c r="E221" s="14">
         <v>6</v>
       </c>
       <c r="F221" s="15">
-        <v>5</v>
-      </c>
-      <c r="G221" s="84"/>
-      <c r="H221" s="99"/>
+        <v>6</v>
+      </c>
+      <c r="G221" s="84" t="s">
+        <v>285</v>
+      </c>
+      <c r="H221" s="99">
+        <v>45169</v>
+      </c>
       <c r="I221" s="98"/>
       <c r="J221" s="80"/>
       <c r="K221" s="1"/>
@@ -8670,12 +8774,22 @@
     </row>
     <row r="222" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="83"/>
-      <c r="B222" s="21"/>
+      <c r="B222" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="C222" s="21"/>
-      <c r="D222" s="21"/>
-      <c r="E222" s="22"/>
-      <c r="F222" s="21"/>
-      <c r="G222" s="99"/>
+      <c r="D222" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E222" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="F222" s="21">
+        <v>0</v>
+      </c>
+      <c r="G222" s="99">
+        <v>45169</v>
+      </c>
       <c r="H222" s="97"/>
       <c r="I222" s="94"/>
       <c r="J222" s="80"/>
@@ -8717,7 +8831,7 @@
         <v>5</v>
       </c>
       <c r="F224" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G224" s="87"/>
       <c r="H224" s="95"/>
@@ -8903,7 +9017,7 @@
         <v>25</v>
       </c>
       <c r="F232" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G232" s="92"/>
       <c r="H232" s="95"/>
@@ -8944,23 +9058,27 @@
     </row>
     <row r="234" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="83"/>
-      <c r="B234" s="28" t="s">
+      <c r="B234" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="C234" s="28" t="s">
+      <c r="C234" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="D234" s="28" t="s">
+      <c r="D234" s="103" t="s">
         <v>213</v>
       </c>
-      <c r="E234" s="29">
+      <c r="E234" s="104">
         <v>12</v>
       </c>
-      <c r="F234" s="30">
-        <v>0</v>
-      </c>
-      <c r="G234" s="92"/>
-      <c r="H234" s="96"/>
+      <c r="F234" s="105">
+        <v>0</v>
+      </c>
+      <c r="G234" s="92" t="s">
+        <v>285</v>
+      </c>
+      <c r="H234" s="96">
+        <v>45162</v>
+      </c>
       <c r="I234" s="94"/>
       <c r="J234" s="1"/>
       <c r="K234" s="1"/>
@@ -8975,18 +9093,20 @@
         <v>19</v>
       </c>
       <c r="C235" s="28" t="s">
-        <v>216</v>
+        <v>319</v>
       </c>
       <c r="D235" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="E235" s="29">
-        <v>1</v>
+        <v>320</v>
+      </c>
+      <c r="E235" s="29" t="s">
+        <v>284</v>
       </c>
       <c r="F235" s="30">
-        <v>2</v>
-      </c>
-      <c r="G235" s="92"/>
+        <v>0</v>
+      </c>
+      <c r="G235" s="92">
+        <v>45162</v>
+      </c>
       <c r="H235" s="96"/>
       <c r="I235" s="94"/>
       <c r="J235" s="80"/>
@@ -9002,16 +9122,16 @@
         <v>19</v>
       </c>
       <c r="C236" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D236" s="28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E236" s="29">
         <v>1</v>
       </c>
       <c r="F236" s="30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G236" s="87"/>
       <c r="H236" s="96"/>
@@ -9025,11 +9145,21 @@
     </row>
     <row r="237" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="83"/>
-      <c r="B237" s="28"/>
-      <c r="C237" s="103"/>
-      <c r="D237" s="103"/>
-      <c r="E237" s="104"/>
-      <c r="F237" s="105"/>
+      <c r="B237" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C237" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="D237" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="E237" s="29">
+        <v>1</v>
+      </c>
+      <c r="F237" s="30">
+        <v>0</v>
+      </c>
       <c r="G237" s="92"/>
       <c r="H237" s="96"/>
       <c r="I237" s="94"/>
@@ -9119,7 +9249,7 @@
       </c>
       <c r="F242" s="38">
         <f>SUM(F224:F241)-SUM(F221:F223)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G242" s="84"/>
       <c r="H242" s="97"/>
@@ -9235,7 +9365,7 @@
         <v>3</v>
       </c>
       <c r="F248" s="15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G248" s="84"/>
       <c r="H248" s="99"/>
@@ -9394,7 +9524,7 @@
         <v>4</v>
       </c>
       <c r="F255" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G255" s="87"/>
       <c r="H255" s="96"/>
@@ -9542,7 +9672,7 @@
         <v>40</v>
       </c>
       <c r="F261" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G261" s="87"/>
       <c r="H261" s="96"/>
@@ -10057,7 +10187,7 @@
         <v>2</v>
       </c>
       <c r="F284" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G284" s="92"/>
       <c r="H284" s="95"/>
@@ -10101,7 +10231,7 @@
         <v>30</v>
       </c>
       <c r="F286" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G286" s="87"/>
       <c r="H286" s="96"/>
@@ -10317,7 +10447,7 @@
       </c>
       <c r="F296" s="38">
         <f>SUM(F277:F295)-SUM(F275:F276)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G296" s="84"/>
       <c r="H296" s="97"/>
@@ -10441,7 +10571,7 @@
         <v>6</v>
       </c>
       <c r="F302" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G302" s="84"/>
       <c r="H302" s="96"/>
@@ -10560,23 +10690,27 @@
     </row>
     <row r="308" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="83"/>
-      <c r="B308" s="28" t="s">
+      <c r="B308" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C308" s="21" t="s">
+      <c r="C308" s="107" t="s">
         <v>253</v>
       </c>
-      <c r="D308" s="21" t="s">
+      <c r="D308" s="107" t="s">
         <v>103</v>
       </c>
-      <c r="E308" s="22">
+      <c r="E308" s="108">
         <v>4</v>
       </c>
       <c r="F308" s="105">
         <v>0</v>
       </c>
-      <c r="G308" s="87"/>
-      <c r="H308" s="95"/>
+      <c r="G308" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="H308" s="96">
+        <v>45169</v>
+      </c>
       <c r="I308" s="95"/>
       <c r="J308" s="1"/>
       <c r="K308" s="1"/>
@@ -10591,18 +10725,20 @@
         <v>18</v>
       </c>
       <c r="C309" s="21" t="s">
-        <v>254</v>
+        <v>322</v>
       </c>
       <c r="D309" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E309" s="22">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="E309" s="22" t="s">
+        <v>284</v>
       </c>
       <c r="F309" s="30">
-        <v>3</v>
-      </c>
-      <c r="G309" s="87"/>
+        <v>0</v>
+      </c>
+      <c r="G309" s="92">
+        <v>45169</v>
+      </c>
       <c r="H309" s="95"/>
       <c r="I309" s="95"/>
       <c r="J309" s="1"/>
@@ -10618,16 +10754,16 @@
         <v>18</v>
       </c>
       <c r="C310" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D310" s="21" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E310" s="22">
         <v>1</v>
       </c>
       <c r="F310" s="30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G310" s="87"/>
       <c r="H310" s="96"/>
@@ -10641,11 +10777,21 @@
     </row>
     <row r="311" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="83"/>
-      <c r="B311" s="28"/>
-      <c r="C311" s="21"/>
-      <c r="D311" s="21"/>
-      <c r="E311" s="22"/>
-      <c r="F311" s="30"/>
+      <c r="B311" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C311" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="D311" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E311" s="22">
+        <v>1</v>
+      </c>
+      <c r="F311" s="30">
+        <v>1</v>
+      </c>
       <c r="G311" s="92"/>
       <c r="H311" s="95"/>
       <c r="I311" s="95"/>
@@ -10715,7 +10861,7 @@
         <v>20</v>
       </c>
       <c r="F314" s="30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G314" s="92"/>
       <c r="H314" s="95"/>
@@ -10783,23 +10929,27 @@
     </row>
     <row r="317" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="83"/>
-      <c r="B317" s="28" t="s">
+      <c r="B317" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="C317" s="21" t="s">
+      <c r="C317" s="107" t="s">
         <v>260</v>
       </c>
-      <c r="D317" s="21" t="s">
+      <c r="D317" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="E317" s="22">
+      <c r="E317" s="108">
         <v>1</v>
       </c>
-      <c r="F317" s="30">
+      <c r="F317" s="105">
         <v>1</v>
       </c>
-      <c r="G317" s="87"/>
-      <c r="H317" s="96"/>
+      <c r="G317" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="H317" s="96">
+        <v>45169</v>
+      </c>
       <c r="I317" s="95"/>
       <c r="J317" s="1"/>
       <c r="K317" s="1"/>
@@ -10810,12 +10960,24 @@
     </row>
     <row r="318" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="83"/>
-      <c r="B318" s="28"/>
-      <c r="C318" s="21"/>
-      <c r="D318" s="21"/>
-      <c r="E318" s="22"/>
-      <c r="F318" s="30"/>
-      <c r="G318" s="92"/>
+      <c r="B318" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C318" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="D318" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E318" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="F318" s="30">
+        <v>0</v>
+      </c>
+      <c r="G318" s="92">
+        <v>45169</v>
+      </c>
       <c r="H318" s="95"/>
       <c r="I318" s="95"/>
       <c r="J318" s="1"/>
@@ -11028,7 +11190,7 @@
         <v>1</v>
       </c>
       <c r="F329" s="15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G329" s="87"/>
       <c r="H329" s="95"/>
@@ -11220,7 +11382,7 @@
         <v>19</v>
       </c>
       <c r="F337" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G337" s="92"/>
       <c r="H337" s="95"/>
@@ -11278,7 +11440,7 @@
         <v>284</v>
       </c>
       <c r="F339" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G339" s="92">
         <v>45155</v>
@@ -11490,7 +11652,7 @@
       </c>
       <c r="F350" s="38">
         <f>SUM(F332:F349)-SUM(F329:F331)</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="G350" s="87"/>
       <c r="H350" s="95"/>
@@ -11560,7 +11722,7 @@
         <v>1</v>
       </c>
       <c r="F356" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="357" spans="2:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -11765,7 +11927,7 @@
         <v>1</v>
       </c>
       <c r="F371" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="372" spans="2:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -11813,7 +11975,7 @@
       </c>
       <c r="F377" s="38">
         <f>SUM(F359:F376)-SUM(F356:F358)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11850,8 +12012,8 @@
   </sheetPr>
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11969,16 +12131,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>301</v>
+        <v>34</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="E7" s="25">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F7" s="26">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G7" s="27">
         <v>2</v>
@@ -11994,19 +12156,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>301</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="E8" s="25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F8" s="26">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G8" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="55"/>
       <c r="I8" s="44"/>
@@ -12025,10 +12187,10 @@
         <v>71</v>
       </c>
       <c r="E9" s="25">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F9" s="26">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G9" s="27">
         <v>7</v>
@@ -12053,10 +12215,10 @@
         <v>4</v>
       </c>
       <c r="F10" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="55"/>
       <c r="I10" s="44"/>
@@ -12078,10 +12240,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G11" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="55"/>
       <c r="I11" s="44"/>
@@ -12091,7 +12253,7 @@
     <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="50"/>
       <c r="B12" s="57">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>46</v>
@@ -12103,10 +12265,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" s="55"/>
       <c r="I12" s="44"/>
@@ -12119,19 +12281,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>224</v>
+        <v>74</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>223</v>
+        <v>84</v>
       </c>
       <c r="E13" s="25">
         <v>2</v>
       </c>
       <c r="F13" s="26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G13" s="27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H13" s="55"/>
       <c r="I13" s="44"/>
@@ -12144,19 +12306,19 @@
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E14" s="25">
         <v>1</v>
       </c>
       <c r="F14" s="59">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G14" s="60">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H14" s="55"/>
       <c r="I14" s="44"/>
@@ -12166,22 +12328,22 @@
     <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50"/>
       <c r="B15" s="57">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="E15" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G15" s="27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H15" s="55"/>
       <c r="I15" s="44"/>
@@ -12191,22 +12353,22 @@
     <row r="16" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="50"/>
       <c r="B16" s="57">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>74</v>
+        <v>224</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="E16" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="26">
         <v>5</v>
       </c>
       <c r="G16" s="27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16" s="55"/>
       <c r="I16" s="44"/>
@@ -12216,7 +12378,7 @@
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="50"/>
       <c r="B17" s="57">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>75</v>
@@ -12228,10 +12390,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G17" s="27">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H17" s="55"/>
       <c r="I17" s="44"/>
@@ -12244,16 +12406,16 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D18" s="61" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E18" s="25">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G18" s="27">
         <v>4</v>
@@ -12269,16 +12431,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E19" s="25">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="F19" s="26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G19" s="27">
         <v>8</v>
@@ -12300,13 +12462,13 @@
         <v>98</v>
       </c>
       <c r="E20" s="25">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="F20" s="26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G20" s="27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H20" s="55"/>
       <c r="I20" s="44"/>

</xml_diff>